<commit_message>
Añadida ronda 6 datos de prueba
</commit_message>
<xml_diff>
--- a/docs/source/_static/Datos de prueba.xlsx
+++ b/docs/source/_static/Datos de prueba.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateo\Desktop\Tabademic-docs\docs\source\_static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7897EB7-8EC3-4D8A-9016-F4D9DBB4B594}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52CD8D58-60BE-4E77-805E-E7BCDA4E3065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="203">
   <si>
     <t>Sala</t>
   </si>
@@ -652,6 +652,9 @@
   </si>
   <si>
     <t>Ronda 5</t>
+  </si>
+  <si>
+    <t>Ronda 6</t>
   </si>
 </sst>
 </file>
@@ -1763,10 +1766,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:K47"/>
+  <dimension ref="A1:L47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D25"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1782,9 +1785,10 @@
     <col min="9" max="9" width="8.88671875" customWidth="1"/>
     <col min="10" max="10" width="13.33203125" customWidth="1"/>
     <col min="11" max="11" width="13.5546875" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>168</v>
       </c>
@@ -1813,13 +1817,16 @@
         <v>201</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>174</v>
+        <v>202</v>
       </c>
       <c r="K1" s="5" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L1" s="5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>176</v>
       </c>
@@ -1849,8 +1856,11 @@
       <c r="K2" s="15" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L2" s="15" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>178</v>
       </c>
@@ -1880,8 +1890,11 @@
       <c r="K3" s="15" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L3" s="15" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>179</v>
       </c>
@@ -1911,8 +1924,11 @@
       <c r="K4" s="15" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L4" s="15" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>180</v>
       </c>
@@ -1942,8 +1958,11 @@
       <c r="K5" s="15" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L5" s="15" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>181</v>
       </c>
@@ -1973,8 +1992,11 @@
       <c r="K6" s="15" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L6" s="15" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>182</v>
       </c>
@@ -2004,8 +2026,11 @@
       <c r="K7" s="15" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L7" s="15" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>183</v>
       </c>
@@ -2035,8 +2060,11 @@
       <c r="K8" s="15" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L8" s="15" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>184</v>
       </c>
@@ -2066,8 +2094,11 @@
       <c r="K9" s="15" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L9" s="15" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>185</v>
       </c>
@@ -2097,8 +2128,11 @@
       <c r="K10" s="15" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L10" s="15" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>186</v>
       </c>
@@ -2128,8 +2162,11 @@
       <c r="K11" s="15" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L11" s="15" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>187</v>
       </c>
@@ -2159,8 +2196,11 @@
       <c r="K12" s="15" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L12" s="15" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>188</v>
       </c>
@@ -2190,8 +2230,11 @@
       <c r="K13" s="15" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L13" s="15" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
         <v>189</v>
       </c>
@@ -2221,8 +2264,11 @@
       <c r="K14" s="15" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L14" s="15" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
         <v>190</v>
       </c>
@@ -2252,8 +2298,11 @@
       <c r="K15" s="15" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L15" s="15" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="12" t="s">
         <v>191</v>
       </c>
@@ -2283,8 +2332,11 @@
       <c r="K16" s="15" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L16" s="15" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="12" t="s">
         <v>192</v>
       </c>
@@ -2314,8 +2366,11 @@
       <c r="K17" s="15" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L17" s="15" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="17" t="s">
         <v>193</v>
       </c>
@@ -2345,8 +2400,11 @@
       <c r="K18" s="15" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L18" s="15" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="12" t="s">
         <v>194</v>
       </c>
@@ -2376,8 +2434,11 @@
       <c r="K19" s="15" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L19" s="15" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="12" t="s">
         <v>195</v>
       </c>
@@ -2407,8 +2468,11 @@
       <c r="K20" s="15" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L20" s="15" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="12" t="s">
         <v>196</v>
       </c>
@@ -2438,8 +2502,11 @@
       <c r="K21" s="15" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L21" s="15" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
         <v>197</v>
       </c>
@@ -2469,8 +2536,11 @@
       <c r="K22" s="15" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L22" s="15" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="12" t="s">
         <v>198</v>
       </c>
@@ -2500,8 +2570,11 @@
       <c r="K23" s="15" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L23" s="15" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="12" t="s">
         <v>199</v>
       </c>
@@ -2531,8 +2604,11 @@
       <c r="K24" s="15" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L24" s="15" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="12" t="s">
         <v>200</v>
       </c>
@@ -2562,8 +2638,11 @@
       <c r="K25" s="15" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L25" s="15" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="18"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -2574,7 +2653,7 @@
       <c r="H26" s="18"/>
       <c r="I26" s="18"/>
     </row>
-    <row r="27" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="18"/>
       <c r="B27" s="18"/>
       <c r="C27" s="18"/>
@@ -2585,7 +2664,7 @@
       <c r="H27" s="18"/>
       <c r="I27" s="18"/>
     </row>
-    <row r="28" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="18"/>
       <c r="B28" s="18"/>
       <c r="C28" s="18"/>
@@ -2596,7 +2675,7 @@
       <c r="H28" s="18"/>
       <c r="I28" s="18"/>
     </row>
-    <row r="29" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="18"/>
       <c r="B29" s="18"/>
       <c r="C29" s="18"/>
@@ -2607,7 +2686,7 @@
       <c r="H29" s="18"/>
       <c r="I29" s="18"/>
     </row>
-    <row r="30" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="18"/>
       <c r="B30" s="18"/>
       <c r="C30" s="18"/>
@@ -2618,7 +2697,7 @@
       <c r="H30" s="18"/>
       <c r="I30" s="18"/>
     </row>
-    <row r="31" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="18"/>
       <c r="B31" s="18"/>
       <c r="C31" s="18"/>
@@ -2629,7 +2708,7 @@
       <c r="H31" s="18"/>
       <c r="I31" s="18"/>
     </row>
-    <row r="32" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="18"/>
       <c r="B32" s="18"/>
       <c r="C32" s="18"/>

</xml_diff>

<commit_message>
Añadidos octavos y cuartos a los datos de prueba
</commit_message>
<xml_diff>
--- a/docs/source/_static/Datos de prueba.xlsx
+++ b/docs/source/_static/Datos de prueba.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateo\Desktop\Tabademic-docs\docs\source\_static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFA86948-79ED-4E4C-A34D-31C1419F4A93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C34FB45C-E67E-4637-A980-21630B470AA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Salas" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="251">
   <si>
     <t>Sala</t>
   </si>
@@ -774,13 +774,19 @@
   </si>
   <si>
     <t>San Basilio</t>
+  </si>
+  <si>
+    <t>Octavos</t>
+  </si>
+  <si>
+    <t>Cuartos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -873,6 +879,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -895,7 +908,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -960,6 +973,12 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1156,7 +1175,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
@@ -2041,10 +2060,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:L47"/>
+  <dimension ref="A1:N47"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2053,17 +2072,16 @@
     <col min="2" max="2" width="16.5546875" style="7" customWidth="1"/>
     <col min="3" max="3" width="25.5546875" style="7" customWidth="1"/>
     <col min="4" max="4" width="21.5546875" style="8" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" customWidth="1"/>
-    <col min="8" max="8" width="9" customWidth="1"/>
-    <col min="9" max="9" width="8.88671875" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" customWidth="1"/>
-    <col min="11" max="11" width="13.5546875" customWidth="1"/>
-    <col min="12" max="12" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" customWidth="1"/>
+    <col min="7" max="7" width="9.77734375" customWidth="1"/>
+    <col min="8" max="9" width="10" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" customWidth="1"/>
+    <col min="11" max="11" width="12.44140625" customWidth="1"/>
+    <col min="12" max="12" width="12.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>167</v>
       </c>
@@ -2095,13 +2113,19 @@
         <v>199</v>
       </c>
       <c r="K1" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="M1" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="N1" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="L1" s="4" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:14" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>175</v>
       </c>
@@ -2134,8 +2158,14 @@
       <c r="L2" s="14" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M2" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="N2" s="26" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>177</v>
       </c>
@@ -2168,8 +2198,14 @@
       <c r="L3" s="14" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M3" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="N3" s="26" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>178</v>
       </c>
@@ -2202,8 +2238,14 @@
       <c r="L4" s="14" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M4" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="N4" s="26" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>179</v>
       </c>
@@ -2236,8 +2278,14 @@
       <c r="L5" s="14" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M5" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="N5" s="26" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>180</v>
       </c>
@@ -2270,8 +2318,14 @@
       <c r="L6" s="14" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M6" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="N6" s="26" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>181</v>
       </c>
@@ -2304,8 +2358,14 @@
       <c r="L7" s="14" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M7" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="N7" s="26" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>182</v>
       </c>
@@ -2338,8 +2398,14 @@
       <c r="L8" s="14" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M8" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="N8" s="26" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="22" t="s">
         <v>203</v>
       </c>
@@ -2372,8 +2438,14 @@
       <c r="L9" s="14" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M9" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="N9" s="26" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>183</v>
       </c>
@@ -2406,8 +2478,14 @@
       <c r="L10" s="14" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M10" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="N10" s="26" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
         <v>184</v>
       </c>
@@ -2440,8 +2518,14 @@
       <c r="L11" s="14" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M11" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="N11" s="26" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>185</v>
       </c>
@@ -2474,8 +2558,14 @@
       <c r="L12" s="14" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M12" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="N12" s="26" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="22" t="s">
         <v>214</v>
       </c>
@@ -2508,8 +2598,14 @@
       <c r="L13" s="14" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M13" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="N13" s="26" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>186</v>
       </c>
@@ -2542,8 +2638,14 @@
       <c r="L14" s="14" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M14" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="N14" s="26" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
         <v>187</v>
       </c>
@@ -2576,8 +2678,14 @@
       <c r="L15" s="14" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M15" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="N15" s="26" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>188</v>
       </c>
@@ -2610,8 +2718,14 @@
       <c r="L16" s="14" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M16" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="N16" s="26" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="22" t="s">
         <v>205</v>
       </c>
@@ -2644,8 +2758,14 @@
       <c r="L17" s="14" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M17" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="N17" s="26" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
         <v>189</v>
       </c>
@@ -2678,8 +2798,14 @@
       <c r="L18" s="14" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M18" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="N18" s="26" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
         <v>190</v>
       </c>
@@ -2712,8 +2838,14 @@
       <c r="L19" s="14" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M19" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="N19" s="26" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
         <v>213</v>
       </c>
@@ -2746,8 +2878,14 @@
       <c r="L20" s="14" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M20" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="N20" s="26" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
         <v>191</v>
       </c>
@@ -2780,8 +2918,14 @@
       <c r="L21" s="14" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M21" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="N21" s="26" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>192</v>
       </c>
@@ -2814,8 +2958,14 @@
       <c r="L22" s="14" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M22" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="N22" s="26" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="22" t="s">
         <v>207</v>
       </c>
@@ -2848,8 +2998,14 @@
       <c r="L23" s="14" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M23" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="N23" s="26" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>193</v>
       </c>
@@ -2882,8 +3038,14 @@
       <c r="L24" s="14" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M24" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="N24" s="26" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
         <v>194</v>
       </c>
@@ -2916,8 +3078,14 @@
       <c r="L25" s="14" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M25" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="N25" s="26" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="22" t="s">
         <v>201</v>
       </c>
@@ -2950,8 +3118,14 @@
       <c r="L26" s="14" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M26" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="N26" s="26" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
         <v>195</v>
       </c>
@@ -2984,8 +3158,14 @@
       <c r="L27" s="14" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M27" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="N27" s="26" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
         <v>200</v>
       </c>
@@ -3018,8 +3198,14 @@
       <c r="L28" s="14" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M28" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="N28" s="26" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
         <v>196</v>
       </c>
@@ -3052,8 +3238,14 @@
       <c r="L29" s="14" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M29" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="N29" s="26" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>197</v>
       </c>
@@ -3086,8 +3278,14 @@
       <c r="L30" s="14" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M30" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="N30" s="26" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="22" t="s">
         <v>209</v>
       </c>
@@ -3120,8 +3318,14 @@
       <c r="L31" s="14" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M31" s="26" t="s">
+        <v>176</v>
+      </c>
+      <c r="N31" s="26" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="16"/>
       <c r="B32" s="16"/>
       <c r="C32" s="16"/>

</xml_diff>

<commit_message>
Añadido el campo Provincia en el éxcel de datos de prueba
</commit_message>
<xml_diff>
--- a/docs/source/_static/Datos de prueba.xlsx
+++ b/docs/source/_static/Datos de prueba.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Salas" sheetId="1" state="visible" r:id="rId3"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="252">
   <si>
     <t xml:space="preserve">Sala</t>
   </si>
@@ -649,6 +649,9 @@
   </si>
   <si>
     <t xml:space="preserve">Juez</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Provincia</t>
   </si>
   <si>
     <t xml:space="preserve">Puntuación</t>
@@ -968,15 +971,15 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1247,7 +1250,7 @@
   </sheetPr>
   <dimension ref="A1:A21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
@@ -1369,7 +1372,7 @@
   </sheetPr>
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -1382,200 +1385,200 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="27.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="28.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="25.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="6" width="20.46"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="7" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="8" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="7" t="s">
+      <c r="C3" s="6"/>
+      <c r="D3" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="8" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="7" t="s">
+      <c r="C4" s="6"/>
+      <c r="D4" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="8" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="7" t="s">
+      <c r="C5" s="6"/>
+      <c r="D5" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="8" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="7" t="s">
+      <c r="C6" s="6"/>
+      <c r="D6" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="8" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="7" t="s">
+      <c r="C7" s="6"/>
+      <c r="D7" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="8" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="7" t="s">
+      <c r="C8" s="6"/>
+      <c r="D8" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="8" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1586,92 +1589,92 @@
       <c r="B9" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="7" t="s">
+      <c r="C9" s="6"/>
+      <c r="D9" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="H9" s="8" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="7" t="s">
+      <c r="C10" s="6"/>
+      <c r="D10" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="H10" s="8" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="7" t="s">
+      <c r="C11" s="6"/>
+      <c r="D11" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="H11" s="8" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="7" t="s">
+      <c r="C12" s="6"/>
+      <c r="D12" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F12" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G12" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="H12" s="7" t="s">
+      <c r="H12" s="8" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1682,92 +1685,92 @@
       <c r="B13" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="7" t="s">
+      <c r="C13" s="6"/>
+      <c r="D13" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="H13" s="7" t="s">
+      <c r="H13" s="8" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="7" t="s">
+      <c r="C14" s="6"/>
+      <c r="D14" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="G14" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="H14" s="7" t="s">
+      <c r="H14" s="8" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="7" t="s">
+      <c r="C15" s="6"/>
+      <c r="D15" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="G15" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="H15" s="7" t="s">
+      <c r="H15" s="8" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="7" t="s">
+      <c r="C16" s="6"/>
+      <c r="D16" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="F16" s="7" t="s">
+      <c r="F16" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="G16" s="7" t="s">
+      <c r="G16" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="H16" s="7" t="s">
+      <c r="H16" s="8" t="s">
         <v>114</v>
       </c>
     </row>
@@ -1778,92 +1781,92 @@
       <c r="B17" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="7" t="s">
+      <c r="C17" s="6"/>
+      <c r="D17" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="G17" s="7" t="s">
+      <c r="G17" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="H17" s="7" t="s">
+      <c r="H17" s="8" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="7" t="s">
+      <c r="C18" s="6"/>
+      <c r="D18" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F18" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="G18" s="7" t="s">
+      <c r="G18" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="H18" s="7" t="s">
+      <c r="H18" s="8" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="7" t="s">
+      <c r="C19" s="6"/>
+      <c r="D19" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="F19" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="G19" s="7" t="s">
+      <c r="G19" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="H19" s="7" t="s">
+      <c r="H19" s="8" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="7" t="s">
+      <c r="C20" s="6"/>
+      <c r="D20" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="F20" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="G20" s="7" t="s">
+      <c r="G20" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="H20" s="7" t="s">
+      <c r="H20" s="8" t="s">
         <v>139</v>
       </c>
     </row>
@@ -1874,44 +1877,44 @@
       <c r="B21" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="7" t="s">
+      <c r="C21" s="6"/>
+      <c r="D21" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="F21" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="G21" s="7" t="s">
+      <c r="G21" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="H21" s="7" t="s">
+      <c r="H21" s="8" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="7" t="s">
+      <c r="C22" s="6"/>
+      <c r="D22" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="E22" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="F22" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="G22" s="7" t="s">
+      <c r="G22" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="H22" s="7" t="s">
+      <c r="H22" s="8" t="s">
         <v>151</v>
       </c>
     </row>
@@ -1922,20 +1925,20 @@
       <c r="B23" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="7" t="s">
+      <c r="C23" s="6"/>
+      <c r="D23" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="E23" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="F23" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="G23" s="7" t="s">
+      <c r="G23" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="H23" s="7" t="s">
+      <c r="H23" s="8" t="s">
         <v>157</v>
       </c>
     </row>
@@ -1946,20 +1949,20 @@
       <c r="B24" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="7" t="s">
+      <c r="C24" s="6"/>
+      <c r="D24" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="E24" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="F24" s="7" t="s">
+      <c r="F24" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="G24" s="7" t="s">
+      <c r="G24" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="H24" s="7" t="s">
+      <c r="H24" s="8" t="s">
         <v>163</v>
       </c>
     </row>
@@ -1970,31 +1973,31 @@
       <c r="B25" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="7" t="s">
+      <c r="C25" s="6"/>
+      <c r="D25" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="E25" s="7" t="s">
+      <c r="E25" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="F25" s="7" t="s">
+      <c r="F25" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="G25" s="7" t="s">
+      <c r="G25" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="H25" s="7" t="s">
+      <c r="H25" s="8" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="8" t="s">
         <v>170</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="C26" s="8"/>
+      <c r="C26" s="6"/>
       <c r="D26" s="1" t="s">
         <v>171</v>
       </c>
@@ -2018,7 +2021,7 @@
       <c r="B27" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="C27" s="8"/>
+      <c r="C27" s="6"/>
       <c r="D27" s="1" t="s">
         <v>177</v>
       </c>
@@ -2036,13 +2039,13 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="8" t="s">
         <v>182</v>
       </c>
       <c r="B28" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="C28" s="8"/>
+      <c r="C28" s="6"/>
       <c r="D28" s="1" t="s">
         <v>184</v>
       </c>
@@ -2066,7 +2069,7 @@
       <c r="B29" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="C29" s="8"/>
+      <c r="C29" s="6"/>
       <c r="D29" s="1" t="s">
         <v>190</v>
       </c>
@@ -2090,7 +2093,7 @@
       <c r="B30" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="C30" s="8"/>
+      <c r="C30" s="6"/>
       <c r="D30" s="1" t="s">
         <v>196</v>
       </c>
@@ -2108,13 +2111,13 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="C31" s="8"/>
+      <c r="C31" s="6"/>
       <c r="D31" s="1" t="s">
         <v>203</v>
       </c>
@@ -2147,1269 +2150,1302 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N47"/>
+  <dimension ref="A1:O47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.55859375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="21.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="21.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="11" width="16.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="11" width="25.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="12" width="21.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="8" width="12.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="8" width="10.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="8" width="9.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="8" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="8" width="11.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="8" width="12.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="8" width="12.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="6" width="14.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="6" width="10.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="6" width="9.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="6" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="6" width="11.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="6" width="12.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="6" width="12.22"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D1" s="13" t="s">
         <v>209</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="13" t="s">
         <v>210</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="7" t="s">
         <v>211</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="14" t="s">
         <v>214</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="M1" s="7" t="s">
         <v>218</v>
       </c>
       <c r="N1" s="15" t="s">
         <v>219</v>
       </c>
+      <c r="O1" s="15" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>24</v>
       </c>
       <c r="C2" s="17"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18" t="s">
-        <v>221</v>
-      </c>
+      <c r="D2" s="0"/>
+      <c r="E2" s="18"/>
       <c r="F2" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="I2" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>222</v>
       </c>
       <c r="J2" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="K2" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="L2" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="M2" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="M2" s="19" t="s">
+        <v>222</v>
       </c>
       <c r="N2" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="O2" s="20" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="16" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>30</v>
       </c>
       <c r="C3" s="17"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18" t="s">
-        <v>221</v>
-      </c>
+      <c r="D3" s="0"/>
+      <c r="E3" s="18"/>
       <c r="F3" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H3" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="I3" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="I3" s="18" t="s">
+        <v>222</v>
       </c>
       <c r="J3" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="K3" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="L3" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="M3" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="M3" s="19" t="s">
+        <v>222</v>
       </c>
       <c r="N3" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="O3" s="20" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="16" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>36</v>
       </c>
       <c r="C4" s="17"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18" t="s">
-        <v>221</v>
-      </c>
+      <c r="D4" s="0"/>
+      <c r="E4" s="18"/>
       <c r="F4" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H4" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="I4" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="I4" s="18" t="s">
+        <v>222</v>
       </c>
       <c r="J4" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="K4" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="L4" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="M4" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="M4" s="19" t="s">
+        <v>222</v>
       </c>
       <c r="N4" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="O4" s="20" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="16" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>42</v>
       </c>
       <c r="C5" s="17"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18" t="s">
-        <v>221</v>
-      </c>
+      <c r="D5" s="0"/>
+      <c r="E5" s="18"/>
       <c r="F5" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="G5" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H5" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="I5" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="I5" s="18" t="s">
+        <v>222</v>
       </c>
       <c r="J5" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="K5" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="L5" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="M5" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="M5" s="19" t="s">
+        <v>222</v>
       </c>
       <c r="N5" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="O5" s="20" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="16" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>48</v>
       </c>
       <c r="C6" s="17"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18" t="s">
-        <v>221</v>
-      </c>
+      <c r="D6" s="0"/>
+      <c r="E6" s="18"/>
       <c r="F6" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H6" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="I6" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="I6" s="18" t="s">
+        <v>222</v>
       </c>
       <c r="J6" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="K6" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="L6" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="M6" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="M6" s="19" t="s">
+        <v>222</v>
       </c>
       <c r="N6" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="O6" s="20" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="16" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>54</v>
       </c>
       <c r="C7" s="17"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18" t="s">
-        <v>221</v>
-      </c>
+      <c r="D7" s="0"/>
+      <c r="E7" s="18"/>
       <c r="F7" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H7" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="I7" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="I7" s="18" t="s">
+        <v>222</v>
       </c>
       <c r="J7" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="K7" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="L7" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="M7" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="M7" s="19" t="s">
+        <v>222</v>
       </c>
       <c r="N7" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="O7" s="20" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="16" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>60</v>
       </c>
       <c r="C8" s="17"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18" t="s">
-        <v>221</v>
-      </c>
+      <c r="D8" s="0"/>
+      <c r="E8" s="18"/>
       <c r="F8" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="G8" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H8" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="I8" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="I8" s="18" t="s">
+        <v>222</v>
       </c>
       <c r="J8" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="K8" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="L8" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="M8" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="M8" s="19" t="s">
+        <v>222</v>
       </c>
       <c r="N8" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="O8" s="20" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="21" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B9" s="21" t="s">
         <v>66</v>
       </c>
       <c r="C9" s="22"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="18" t="s">
-        <v>221</v>
-      </c>
+      <c r="D9" s="0"/>
+      <c r="E9" s="23"/>
       <c r="F9" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H9" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="I9" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="I9" s="18" t="s">
+        <v>222</v>
       </c>
       <c r="J9" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="K9" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="L9" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="M9" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="M9" s="19" t="s">
+        <v>222</v>
       </c>
       <c r="N9" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="O9" s="20" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="16" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>72</v>
       </c>
       <c r="C10" s="17"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18" t="s">
-        <v>221</v>
-      </c>
+      <c r="D10" s="0"/>
+      <c r="E10" s="18"/>
       <c r="F10" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H10" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="I10" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="I10" s="18" t="s">
+        <v>222</v>
       </c>
       <c r="J10" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="K10" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="L10" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="M10" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="M10" s="19" t="s">
+        <v>222</v>
       </c>
       <c r="N10" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="O10" s="20" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="16" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>78</v>
       </c>
       <c r="C11" s="17"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18" t="s">
-        <v>221</v>
-      </c>
+      <c r="D11" s="0"/>
+      <c r="E11" s="18"/>
       <c r="F11" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H11" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="I11" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="I11" s="18" t="s">
+        <v>222</v>
       </c>
       <c r="J11" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="K11" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="L11" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="M11" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="M11" s="19" t="s">
+        <v>222</v>
       </c>
       <c r="N11" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="O11" s="20" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="16" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>84</v>
       </c>
       <c r="C12" s="17"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18" t="s">
-        <v>221</v>
-      </c>
+      <c r="D12" s="0"/>
+      <c r="E12" s="18"/>
       <c r="F12" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="G12" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H12" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="I12" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="I12" s="18" t="s">
+        <v>222</v>
       </c>
       <c r="J12" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="K12" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="L12" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="M12" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="M12" s="19" t="s">
+        <v>222</v>
       </c>
       <c r="N12" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="O12" s="20" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="21" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B13" s="21" t="s">
         <v>91</v>
       </c>
       <c r="C13" s="22"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="18" t="s">
-        <v>221</v>
-      </c>
+      <c r="D13" s="0"/>
+      <c r="E13" s="23"/>
       <c r="F13" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="G13" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H13" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="I13" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="I13" s="18" t="s">
+        <v>222</v>
       </c>
       <c r="J13" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="K13" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="L13" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="M13" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="M13" s="19" t="s">
+        <v>222</v>
       </c>
       <c r="N13" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="O13" s="20" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="16" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>97</v>
       </c>
       <c r="C14" s="17"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18" t="s">
-        <v>221</v>
-      </c>
+      <c r="D14" s="0"/>
+      <c r="E14" s="18"/>
       <c r="F14" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="G14" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H14" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="I14" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="I14" s="18" t="s">
+        <v>222</v>
       </c>
       <c r="J14" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="K14" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="L14" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="M14" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="M14" s="19" t="s">
+        <v>222</v>
       </c>
       <c r="N14" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="O14" s="20" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="16" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>103</v>
       </c>
       <c r="C15" s="17"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18" t="s">
-        <v>221</v>
-      </c>
+      <c r="D15" s="0"/>
+      <c r="E15" s="18"/>
       <c r="F15" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="G15" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H15" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="I15" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="I15" s="18" t="s">
+        <v>222</v>
       </c>
       <c r="J15" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="K15" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="L15" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="M15" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="M15" s="19" t="s">
+        <v>222</v>
       </c>
       <c r="N15" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="O15" s="20" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="16" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>109</v>
       </c>
       <c r="C16" s="17"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18" t="s">
-        <v>221</v>
-      </c>
+      <c r="D16" s="0"/>
+      <c r="E16" s="18"/>
       <c r="F16" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="G16" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H16" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="I16" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="I16" s="18" t="s">
+        <v>222</v>
       </c>
       <c r="J16" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="K16" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="L16" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="M16" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="M16" s="19" t="s">
+        <v>222</v>
       </c>
       <c r="N16" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="O16" s="20" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="21" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B17" s="21" t="s">
         <v>116</v>
       </c>
       <c r="C17" s="22"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="18" t="s">
-        <v>221</v>
-      </c>
+      <c r="D17" s="0"/>
+      <c r="E17" s="23"/>
       <c r="F17" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="G17" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H17" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="I17" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="I17" s="18" t="s">
+        <v>222</v>
       </c>
       <c r="J17" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="K17" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="L17" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="M17" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="M17" s="19" t="s">
+        <v>222</v>
       </c>
       <c r="N17" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="O17" s="20" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="16" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>122</v>
       </c>
       <c r="C18" s="17"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18" t="s">
-        <v>221</v>
-      </c>
+      <c r="D18" s="0"/>
+      <c r="E18" s="18"/>
       <c r="F18" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="G18" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H18" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="I18" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="I18" s="18" t="s">
+        <v>222</v>
       </c>
       <c r="J18" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="K18" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="L18" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="M18" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="M18" s="19" t="s">
+        <v>222</v>
       </c>
       <c r="N18" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="O18" s="20" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="16" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>128</v>
       </c>
       <c r="C19" s="17"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18" t="s">
-        <v>221</v>
-      </c>
+      <c r="D19" s="0"/>
+      <c r="E19" s="18"/>
       <c r="F19" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="G19" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H19" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="I19" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="I19" s="18" t="s">
+        <v>222</v>
       </c>
       <c r="J19" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="K19" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="L19" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="M19" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="M19" s="19" t="s">
+        <v>222</v>
       </c>
       <c r="N19" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="O19" s="20" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="16" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B20" s="24" t="s">
         <v>202</v>
       </c>
       <c r="C20" s="17"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18" t="s">
-        <v>221</v>
-      </c>
+      <c r="D20" s="0"/>
+      <c r="E20" s="18"/>
       <c r="F20" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="G20" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H20" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="I20" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="I20" s="18" t="s">
+        <v>222</v>
       </c>
       <c r="J20" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="K20" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="L20" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="M20" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="M20" s="19" t="s">
+        <v>222</v>
       </c>
       <c r="N20" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="O20" s="20" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="16" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>183</v>
       </c>
       <c r="C21" s="17"/>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18" t="s">
-        <v>221</v>
-      </c>
+      <c r="D21" s="0"/>
+      <c r="E21" s="18"/>
       <c r="F21" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="G21" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H21" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="I21" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="I21" s="18" t="s">
+        <v>222</v>
       </c>
       <c r="J21" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="K21" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="L21" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="M21" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="M21" s="19" t="s">
+        <v>222</v>
       </c>
       <c r="N21" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="O21" s="20" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="16" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>134</v>
       </c>
       <c r="C22" s="17"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18" t="s">
-        <v>221</v>
-      </c>
+      <c r="D22" s="0"/>
+      <c r="E22" s="18"/>
       <c r="F22" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="G22" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H22" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="I22" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="I22" s="18" t="s">
+        <v>222</v>
       </c>
       <c r="J22" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="K22" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="L22" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="M22" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="M22" s="19" t="s">
+        <v>222</v>
       </c>
       <c r="N22" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="O22" s="20" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="21" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B23" s="21" t="s">
         <v>140</v>
       </c>
       <c r="C23" s="22"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="18" t="s">
-        <v>221</v>
-      </c>
+      <c r="D23" s="0"/>
+      <c r="E23" s="23"/>
       <c r="F23" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="G23" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H23" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="I23" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="I23" s="18" t="s">
+        <v>222</v>
       </c>
       <c r="J23" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="K23" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="L23" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="M23" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="M23" s="19" t="s">
+        <v>222</v>
       </c>
       <c r="N23" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="O23" s="20" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="16" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B24" s="9" t="s">
         <v>146</v>
       </c>
       <c r="C24" s="17"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18" t="s">
-        <v>221</v>
-      </c>
+      <c r="D24" s="0"/>
+      <c r="E24" s="18"/>
       <c r="F24" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="G24" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H24" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="I24" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="I24" s="18" t="s">
+        <v>222</v>
       </c>
       <c r="J24" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="K24" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="L24" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="M24" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="M24" s="19" t="s">
+        <v>222</v>
       </c>
       <c r="N24" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="O24" s="20" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="16" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B25" s="24" t="s">
         <v>152</v>
       </c>
       <c r="C25" s="17"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18" t="s">
-        <v>221</v>
-      </c>
+      <c r="D25" s="0"/>
+      <c r="E25" s="18"/>
       <c r="F25" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="G25" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H25" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="I25" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="I25" s="18" t="s">
+        <v>222</v>
       </c>
       <c r="J25" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="K25" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="L25" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="M25" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="M25" s="19" t="s">
+        <v>222</v>
       </c>
       <c r="N25" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="O25" s="20" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="21" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B26" s="21" t="s">
         <v>158</v>
       </c>
       <c r="C26" s="5"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="18" t="s">
-        <v>221</v>
-      </c>
+      <c r="D26" s="0"/>
+      <c r="E26" s="23"/>
       <c r="F26" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="G26" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H26" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="I26" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="I26" s="18" t="s">
+        <v>222</v>
       </c>
       <c r="J26" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="K26" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="L26" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="M26" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="M26" s="19" t="s">
+        <v>222</v>
       </c>
       <c r="N26" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="O26" s="20" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="16" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B27" s="24" t="s">
         <v>164</v>
       </c>
       <c r="C27" s="17"/>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18" t="s">
-        <v>221</v>
-      </c>
+      <c r="D27" s="0"/>
+      <c r="E27" s="18"/>
       <c r="F27" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="G27" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H27" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="I27" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="I27" s="18" t="s">
+        <v>222</v>
       </c>
       <c r="J27" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="K27" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="L27" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="M27" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="M27" s="19" t="s">
+        <v>222</v>
       </c>
       <c r="N27" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="O27" s="20" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="16" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B28" s="24" t="s">
         <v>170</v>
       </c>
       <c r="C28" s="17"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18" t="s">
-        <v>221</v>
-      </c>
+      <c r="D28" s="0"/>
+      <c r="E28" s="18"/>
       <c r="F28" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="G28" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H28" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="I28" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="I28" s="18" t="s">
+        <v>222</v>
       </c>
       <c r="J28" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="K28" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="L28" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="M28" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="M28" s="19" t="s">
+        <v>222</v>
       </c>
       <c r="N28" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="O28" s="20" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="16" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B29" s="24" t="s">
         <v>176</v>
       </c>
       <c r="C29" s="17"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18" t="s">
-        <v>221</v>
-      </c>
+      <c r="D29" s="0"/>
+      <c r="E29" s="18"/>
       <c r="F29" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="G29" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H29" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="I29" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="I29" s="18" t="s">
+        <v>222</v>
       </c>
       <c r="J29" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="K29" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="L29" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="M29" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="M29" s="19" t="s">
+        <v>222</v>
       </c>
       <c r="N29" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="O29" s="20" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="16" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B30" s="24" t="s">
         <v>189</v>
       </c>
       <c r="C30" s="17"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18" t="s">
-        <v>221</v>
-      </c>
+      <c r="D30" s="0"/>
+      <c r="E30" s="18"/>
       <c r="F30" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="G30" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H30" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="I30" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="I30" s="18" t="s">
+        <v>222</v>
       </c>
       <c r="J30" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="K30" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="L30" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="M30" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="M30" s="19" t="s">
+        <v>222</v>
       </c>
       <c r="N30" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="O30" s="20" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="21" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B31" s="21" t="s">
         <v>195</v>
       </c>
       <c r="C31" s="22"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="18" t="s">
-        <v>221</v>
-      </c>
+      <c r="D31" s="0"/>
+      <c r="E31" s="23"/>
       <c r="F31" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="G31" s="18" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H31" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="I31" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="I31" s="18" t="s">
+        <v>222</v>
       </c>
       <c r="J31" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="K31" s="19" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="L31" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="M31" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="M31" s="19" t="s">
+        <v>222</v>
       </c>
       <c r="N31" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
+      </c>
+      <c r="O31" s="20" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Renombre salas éxcel prueba
</commit_message>
<xml_diff>
--- a/docs/source/_static/Datos de prueba.xlsx
+++ b/docs/source/_static/Datos de prueba.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Salas" sheetId="1" state="visible" r:id="rId3"/>
@@ -22,54 +22,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="238">
   <si>
     <t xml:space="preserve">Sala</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alcázar de los Reyes Cristianos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Caballerizas Reales</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calleja de las Flores</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Iglesia de Santa Marina</t>
-  </si>
-  <si>
-    <t xml:space="preserve">La Judería</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medina Azahara</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mezquita-Catedral</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Palacio de Viana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plaza de Capuchinos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plaza de la Corredera</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plaza de las Tendillas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Puente Romano</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Puerta de Almodóvar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">San Basilio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Torre de la Calahorra</t>
   </si>
   <si>
     <t xml:space="preserve">Equipo</t>
@@ -963,11 +918,11 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -1072,31 +1027,6 @@
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF0000FF"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
 </styleSheet>
 </file>
 
@@ -1278,8 +1208,8 @@
   </sheetPr>
   <dimension ref="A1:A21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.55859375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1293,77 +1223,77 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="3" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="4" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="3" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="3" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="4" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="3" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="4" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="3" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="4" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="n">
         <v>11</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="4" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="3" t="n">
         <v>13</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="4" t="n">
         <v>14</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="3" t="n">
         <v>15</v>
       </c>
     </row>
@@ -1418,748 +1348,748 @@
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="8" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="8" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="8" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="8" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="8" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="8" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="8" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="8" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="8" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="8" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="8" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="8" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="8" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="8" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="8" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="8" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="9" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="8" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="8" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="8" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="C19" s="6"/>
       <c r="D19" s="8" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="8" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="8" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="9" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="8" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="C22" s="6"/>
       <c r="D22" s="8" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="8" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="8" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="10" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="C24" s="6"/>
       <c r="D24" s="8" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="10" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="C25" s="6"/>
       <c r="D25" s="1" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="8" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="C26" s="6"/>
       <c r="D26" s="1" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="10" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="C27" s="6"/>
       <c r="D27" s="1" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="8" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="C28" s="6"/>
       <c r="D28" s="1" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="17.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="10" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="C29" s="6"/>
       <c r="D29" s="1" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="9" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="C30" s="6"/>
       <c r="D30" s="1" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="8" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="C31" s="6"/>
       <c r="D31" s="6" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -2180,7 +2110,7 @@
   </sheetPr>
   <dimension ref="A1:O47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -2197,1284 +2127,1284 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="6" width="11.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="6" width="12.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="6" width="12.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="12.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="6" width="12.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="7" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="N1" s="15" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
       <c r="O1" s="15" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="16" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="C2" s="17"/>
       <c r="D2" s="6"/>
       <c r="E2" s="18"/>
       <c r="F2" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="J2" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="K2" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="L2" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="M2" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="N2" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="O2" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="16" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C3" s="17"/>
       <c r="D3" s="6"/>
       <c r="E3" s="18"/>
       <c r="F3" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="G3" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="H3" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="I3" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="J3" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="K3" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="L3" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="M3" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="N3" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="O3" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="16" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="C4" s="17"/>
       <c r="D4" s="6"/>
       <c r="E4" s="18"/>
       <c r="F4" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="H4" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="I4" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="J4" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="K4" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="L4" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="M4" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="N4" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="O4" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="16" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="C5" s="17"/>
       <c r="D5" s="6"/>
       <c r="E5" s="18"/>
       <c r="F5" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="G5" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="H5" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="I5" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="J5" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="K5" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="L5" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="M5" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="N5" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="O5" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="16" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="C6" s="17"/>
       <c r="D6" s="6"/>
       <c r="E6" s="18"/>
       <c r="F6" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="H6" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="I6" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="J6" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="K6" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="L6" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="M6" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="N6" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="O6" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="16" t="s">
-        <v>228</v>
+        <v>213</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="C7" s="17"/>
       <c r="D7" s="6"/>
       <c r="E7" s="18"/>
       <c r="F7" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="H7" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="I7" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="J7" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="K7" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="L7" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="M7" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="N7" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="O7" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="16" t="s">
-        <v>229</v>
+        <v>214</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="C8" s="17"/>
       <c r="D8" s="6"/>
       <c r="E8" s="18"/>
       <c r="F8" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="G8" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="H8" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="I8" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="J8" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="K8" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="L8" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="M8" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="N8" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="O8" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="21" t="s">
-        <v>230</v>
+        <v>215</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="C9" s="22"/>
       <c r="D9" s="6"/>
       <c r="E9" s="23"/>
       <c r="F9" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="G9" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="H9" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="I9" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="J9" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="K9" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="L9" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="M9" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="N9" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="O9" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="16" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="C10" s="17"/>
       <c r="D10" s="6"/>
       <c r="E10" s="18"/>
       <c r="F10" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="G10" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="H10" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="I10" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="J10" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="K10" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="L10" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="M10" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="N10" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="O10" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="16" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="C11" s="17"/>
       <c r="D11" s="6"/>
       <c r="E11" s="18"/>
       <c r="F11" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="G11" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="H11" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="I11" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="J11" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="K11" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="L11" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="M11" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="N11" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="O11" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="16" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="C12" s="17"/>
       <c r="D12" s="6"/>
       <c r="E12" s="18"/>
       <c r="F12" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="G12" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="H12" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="I12" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="J12" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="K12" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="L12" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="M12" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="N12" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="O12" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="21" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="C13" s="22"/>
       <c r="D13" s="6"/>
       <c r="E13" s="23"/>
       <c r="F13" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="G13" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="H13" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="I13" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="J13" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="K13" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="L13" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="M13" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="N13" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="O13" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="16" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="C14" s="17"/>
       <c r="D14" s="6"/>
       <c r="E14" s="18"/>
       <c r="F14" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="G14" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="H14" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="I14" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="J14" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="K14" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="L14" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="M14" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="N14" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="O14" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="16" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="C15" s="17"/>
       <c r="D15" s="6"/>
       <c r="E15" s="18"/>
       <c r="F15" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="G15" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="H15" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="I15" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="J15" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="K15" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="L15" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="M15" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="N15" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="O15" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="16" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="C16" s="17"/>
       <c r="D16" s="6"/>
       <c r="E16" s="18"/>
       <c r="F16" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="G16" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="H16" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="I16" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="J16" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="K16" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="L16" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="M16" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="N16" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="O16" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="21" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="C17" s="22"/>
       <c r="D17" s="6"/>
       <c r="E17" s="23"/>
       <c r="F17" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="G17" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="H17" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="I17" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="J17" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="K17" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="L17" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="M17" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="N17" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="O17" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="16" t="s">
-        <v>239</v>
+        <v>224</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="C18" s="17"/>
       <c r="D18" s="6"/>
       <c r="E18" s="18"/>
       <c r="F18" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="G18" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="H18" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="I18" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="J18" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="K18" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="L18" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="M18" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="N18" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="O18" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="16" t="s">
-        <v>240</v>
+        <v>225</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="C19" s="17"/>
       <c r="D19" s="6"/>
       <c r="E19" s="18"/>
       <c r="F19" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="G19" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="H19" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="I19" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="J19" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="K19" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="L19" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="M19" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="N19" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="O19" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="16" t="s">
-        <v>241</v>
+        <v>226</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="C20" s="17"/>
       <c r="D20" s="6"/>
       <c r="E20" s="18"/>
       <c r="F20" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="G20" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="H20" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="I20" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="J20" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="K20" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="L20" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="M20" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="N20" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="O20" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="16" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="C21" s="17"/>
       <c r="D21" s="6"/>
       <c r="E21" s="18"/>
       <c r="F21" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="G21" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="H21" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="I21" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="J21" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="K21" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="L21" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="M21" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="N21" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="O21" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="16" t="s">
-        <v>243</v>
+        <v>228</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="C22" s="17"/>
       <c r="D22" s="6"/>
       <c r="E22" s="18"/>
       <c r="F22" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="G22" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="H22" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="I22" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="J22" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="K22" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="L22" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="M22" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="N22" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="O22" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="21" t="s">
-        <v>244</v>
+        <v>229</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="6"/>
       <c r="E23" s="23"/>
       <c r="F23" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="G23" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="H23" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="I23" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="J23" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="K23" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="L23" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="M23" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="N23" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="O23" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="21" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="C24" s="22"/>
       <c r="D24" s="6"/>
       <c r="E24" s="23"/>
       <c r="F24" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="G24" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="H24" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="I24" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="J24" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="K24" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="L24" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="M24" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="N24" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="O24" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="16" t="s">
-        <v>246</v>
+        <v>231</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="C25" s="17"/>
       <c r="D25" s="6"/>
       <c r="E25" s="18"/>
       <c r="F25" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="G25" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="H25" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="I25" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="J25" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="K25" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="L25" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="M25" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="N25" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="O25" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="16" t="s">
-        <v>247</v>
+        <v>232</v>
       </c>
       <c r="B26" s="24" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="C26" s="17"/>
       <c r="D26" s="6"/>
       <c r="E26" s="18"/>
       <c r="F26" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="G26" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="H26" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="I26" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="J26" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="K26" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="L26" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="M26" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="N26" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="O26" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="16" t="s">
-        <v>248</v>
+        <v>233</v>
       </c>
       <c r="B27" s="24" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="C27" s="17"/>
       <c r="D27" s="6"/>
       <c r="E27" s="18"/>
       <c r="F27" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="G27" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="H27" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="I27" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="J27" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="K27" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="L27" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="M27" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="N27" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="O27" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="16" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="B28" s="24" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="C28" s="17"/>
       <c r="D28" s="6"/>
       <c r="E28" s="18"/>
       <c r="F28" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="G28" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="H28" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="I28" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="J28" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="K28" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="L28" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="M28" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="N28" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="O28" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="16" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
       <c r="B29" s="24" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="C29" s="17"/>
       <c r="D29" s="6"/>
       <c r="E29" s="18"/>
       <c r="F29" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="G29" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="H29" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="I29" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="J29" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="K29" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="L29" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="M29" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="N29" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="O29" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="16" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
       <c r="B30" s="24" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="C30" s="17"/>
       <c r="D30" s="6"/>
       <c r="E30" s="18"/>
       <c r="F30" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="G30" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="H30" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="I30" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="J30" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="K30" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="L30" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="M30" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="N30" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="O30" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="21" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
       <c r="B31" s="21" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="C31" s="22"/>
       <c r="D31" s="6"/>
       <c r="E31" s="23"/>
       <c r="F31" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="G31" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="H31" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="I31" s="18" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="J31" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="K31" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="L31" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="M31" s="19" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="N31" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="O31" s="20" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>